<commit_message>
Carat: Bug fix iteration
</commit_message>
<xml_diff>
--- a/Carat/templates/LoadBySubjects.xlsx
+++ b/Carat/templates/LoadBySubjects.xlsx
@@ -22,16 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Робота
-в ДЕК</t>
   </si>
   <si>
     <t>Екзамени</t>
@@ -68,36 +64,6 @@
     <t>(повна назва кафедри)</t>
   </si>
   <si>
-    <t>магістрів</t>
-  </si>
-  <si>
-    <t>магістрів</t>
-  </si>
-  <si>
-    <t>магістрів</t>
-  </si>
-  <si>
-    <t>магістрів</t>
-  </si>
-  <si>
-    <t>магістрів</t>
-  </si>
-  <si>
-    <t>спеціалістів</t>
-  </si>
-  <si>
-    <t>спеціалістів</t>
-  </si>
-  <si>
-    <t>спеціалістів</t>
-  </si>
-  <si>
-    <t>спеціалістів</t>
-  </si>
-  <si>
-    <t>спеціалістів</t>
-  </si>
-  <si>
     <t>№ п/п</t>
   </si>
   <si>
@@ -124,9 +90,6 @@
 атестац. роб</t>
   </si>
   <si>
-    <t>Практич.заняття (семін.)</t>
-  </si>
-  <si>
     <t>Керівництво</t>
   </si>
   <si>
@@ -179,9 +142,6 @@
     <t>Курсові роботи</t>
   </si>
   <si>
-    <t>Консультування по державному екзамену</t>
-  </si>
-  <si>
     <t>Реферати</t>
   </si>
   <si>
@@ -189,13 +149,34 @@
   </si>
   <si>
     <t>II семестр, бюджет, денна форма навчання</t>
+  </si>
+  <si>
+    <t>Практич.заняття
+(комп. практик. семін.)</t>
+  </si>
+  <si>
+    <t>за змішаною
+формою начвання</t>
+  </si>
+  <si>
+    <t>магістр ОПП</t>
+  </si>
+  <si>
+    <t>магістр ОНП</t>
+  </si>
+  <si>
+    <t>Вступний іспит</t>
+  </si>
+  <si>
+    <t>Робота
+в ЕК</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -251,6 +232,17 @@
       <name val="Arial Cyr"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial Cyr"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial Cyr"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -260,7 +252,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -385,11 +377,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -445,6 +448,24 @@
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -458,30 +479,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +794,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL46"/>
+  <dimension ref="A1:AM46"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -778,35 +805,35 @@
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="2.85546875" customWidth="1"/>
-    <col min="4" max="37" width="6.7109375" customWidth="1"/>
+    <col min="4" max="38" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="13"/>
+      <c r="AC2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="Z2" s="13"/>
-      <c r="AB2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B3" s="14" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="12" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -828,12 +855,13 @@
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="12"/>
-      <c r="Y3" s="10"/>
-      <c r="AB3" s="3"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="10"/>
+      <c r="AC3" s="3"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -866,7 +894,7 @@
       <c r="AD4" s="13"/>
       <c r="AE4" s="13"/>
     </row>
-    <row r="5" spans="1:38" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -898,184 +926,189 @@
       <c r="AC5" s="13"/>
       <c r="AD5" s="13"/>
       <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:38" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:39" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="D7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="42"/>
+      <c r="AC7" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD7" s="43"/>
+      <c r="AE7" s="43"/>
+      <c r="AF7" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="AG7" s="25"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ7" s="25"/>
+      <c r="AK7" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL7" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM7" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7" s="22" t="s">
+      <c r="R8" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="39"/>
+      <c r="T8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="X8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y8" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="N7" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="O7" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="P7" s="33" t="s">
+      <c r="AD8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE8" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH8" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC7" s="27"/>
-      <c r="AD7" s="27"/>
-      <c r="AE7" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
-      <c r="AH7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI7" s="27"/>
-      <c r="AJ7" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK7" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL7" s="30" t="s">
-        <v>26</v>
-      </c>
+      <c r="AK8" s="37"/>
+      <c r="AL8" s="37"/>
+      <c r="AM8" s="35"/>
     </row>
-    <row r="8" spans="1:38" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="R8" s="32"/>
-      <c r="S8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="W8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ8" s="32"/>
-      <c r="AK8" s="31"/>
-      <c r="AL8" s="30"/>
-    </row>
-    <row r="9" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="9"/>
       <c r="C9" s="16"/>
@@ -1113,12 +1146,13 @@
       <c r="AI9" s="17"/>
       <c r="AJ9" s="17"/>
       <c r="AK9" s="17"/>
-      <c r="AL9" s="18"/>
+      <c r="AL9" s="17"/>
+      <c r="AM9" s="18"/>
     </row>
-    <row r="10" spans="1:38" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="15" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="20">
@@ -1126,180 +1160,173 @@
         <v>0</v>
       </c>
       <c r="E10" s="20">
-        <f>SUM(E9:E9)</f>
+        <f t="shared" ref="E10:AL10" si="0">SUM(E9:E9)</f>
         <v>0</v>
       </c>
       <c r="F10" s="20">
-        <f>SUM(F9:F9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G10" s="20">
-        <f>SUM(G9:G9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="20">
-        <f>SUM(H9:H9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I10" s="20">
-        <f>SUM(I9:I9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J10" s="20">
-        <f>SUM(J9:J9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10" s="20">
-        <f>SUM(K9:K9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L10" s="20">
-        <f>SUM(L9:L9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M10" s="20">
-        <f>SUM(M9:M9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10" s="20">
-        <f>SUM(N9:N9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O10" s="20">
-        <f>SUM(O9:O9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P10" s="20">
-        <f>SUM(P9:P9)</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="20">
-        <f>SUM(Q9:Q9)</f>
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="20"/>
       <c r="R10" s="20">
-        <f>SUM(R9:R9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S10" s="20">
-        <f>SUM(S9:S9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T10" s="20">
-        <f>SUM(T9:T9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U10" s="20">
-        <f>SUM(U9:U9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V10" s="20">
-        <f>SUM(V9:V9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W10" s="20">
-        <f>SUM(W9:W9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X10" s="20">
-        <f>SUM(X9:X9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y10" s="20">
-        <f>SUM(Y9:Y9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z10" s="20">
-        <f>SUM(Z9:Z9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA10" s="20">
-        <f>SUM(AA9:AA9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB10" s="20">
-        <f>SUM(AB9:AB9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC10" s="20">
-        <f>SUM(AC9:AC9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD10" s="20">
-        <f>SUM(AD9:AD9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE10" s="20">
-        <f>SUM(AE9:AE9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF10" s="20">
-        <f>SUM(AF9:AF9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG10" s="20">
-        <f>SUM(AG9:AG9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH10" s="20">
-        <f>SUM(AH9:AH9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI10" s="20">
-        <f>SUM(AI9:AI9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ10" s="20">
-        <f>SUM(AJ9:AJ9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK10" s="20">
-        <f>SUM(AK9:AK9)</f>
-        <v>0</v>
-      </c>
-      <c r="AL10" s="21">
-        <f t="shared" ref="AL10" si="0">SUM(D10:AK10)</f>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL10" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AM10" s="21">
+        <f t="shared" ref="AM10" si="1">SUM(D10:AL10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="AF11" s="7"/>
-      <c r="AG11" s="6"/>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AG11" s="7"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="AF12" s="6"/>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="AG12" s="6"/>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
+      <c r="AJ12" s="6"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="AF13" s="6"/>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="AG13" s="6"/>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
+      <c r="AJ13" s="6"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="AF14" s="6"/>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="AG14" s="6"/>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
     </row>
     <row r="46" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AL7:AL8"/>
-    <mergeCell ref="AJ7:AJ8"/>
-    <mergeCell ref="AK7:AK8"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Y7:AA7"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="N7:N8"/>
@@ -1312,13 +1339,21 @@
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="AK7:AK8"/>
+    <mergeCell ref="AL7:AL8"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="AC7:AE7"/>
+    <mergeCell ref="Z7:AB7"/>
+    <mergeCell ref="AF7:AH7"/>
+    <mergeCell ref="AI7:AJ7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.19685039370078741" bottom="0.39370078740157483" header="0" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="63" fitToHeight="10" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="63" fitToHeight="10" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;R&amp;P</oddFooter>
   </headerFooter>

</xml_diff>